<commit_message>
LOOKUPTABLE change for resistor rules
</commit_message>
<xml_diff>
--- a/LOOKUPTABLE.xlsx
+++ b/LOOKUPTABLE.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\배포용_BOM 디레이팅 프로그램\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yohan Choi\Desktop\EMT_Derating\EMT_Derating_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5888B77D-9A34-4DCF-9F13-6D5E5D5F3DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CAB5AA-CF62-4BA9-B828-8C32E3579A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{5D39A059-4D80-4698-A944-9977A2F81BBD}"/>
+    <workbookView xWindow="-16320" yWindow="-6540" windowWidth="16440" windowHeight="28320" xr2:uid="{5D39A059-4D80-4698-A944-9977A2F81BBD}"/>
   </bookViews>
   <sheets>
-    <sheet name="TABLE" sheetId="1" r:id="rId1"/>
-    <sheet name="ROUTING_RULES" sheetId="2" r:id="rId2"/>
+    <sheet name="RESISTOR_PREFIX" sheetId="3" r:id="rId1"/>
+    <sheet name="TABLE" sheetId="1" r:id="rId2"/>
+    <sheet name="ROUTING_RULES" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="206">
   <si>
     <t>Category</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -681,6 +682,48 @@
   <si>
     <t>XC6223H181MR-G</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefix</t>
+  </si>
+  <si>
+    <t>Rating_Value</t>
+  </si>
+  <si>
+    <t>Rating_Unit</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>WR02X</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>WALSIN</t>
+  </si>
+  <si>
+    <t>WR04X</t>
+  </si>
+  <si>
+    <t>WR06X</t>
+  </si>
+  <si>
+    <t>CRCW0</t>
+  </si>
+  <si>
+    <t>VISHAY</t>
+  </si>
+  <si>
+    <t>ERJ2G</t>
+  </si>
+  <si>
+    <t>PANASONIC</t>
   </si>
 </sst>
 </file>
@@ -774,9 +817,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -814,7 +857,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -920,7 +963,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1062,17 +1105,133 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08DFA35F-C35F-402D-A757-AEE3B3DD27ED}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2">
+        <v>0.1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3">
+        <v>0.125</v>
+      </c>
+      <c r="C3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4">
+        <v>0.25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B5">
+        <v>0.1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B6">
+        <v>0.1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D6" t="s">
+        <v>205</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71CCCFF0-23C6-49D1-B575-F0E9EDED363D}">
   <dimension ref="A1:F184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+    <sheetView topLeftCell="A166" workbookViewId="0">
       <selection activeCell="G154" sqref="G154"/>
     </sheetView>
   </sheetViews>
@@ -4379,7 +4538,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD55E4DB-5EAD-49B0-BD30-E39360F35C86}">
   <dimension ref="A1:C6"/>
   <sheetViews>

</xml_diff>

<commit_message>
Walsin resistor rule modified
</commit_message>
<xml_diff>
--- a/LOOKUPTABLE.xlsx
+++ b/LOOKUPTABLE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yohan Choi\Desktop\EMT_Derating\EMT_Derating_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CAB5AA-CF62-4BA9-B828-8C32E3579A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD9D59C-C900-4792-A6ED-25BB012298F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-6540" windowWidth="16440" windowHeight="28320" xr2:uid="{5D39A059-4D80-4698-A944-9977A2F81BBD}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="206">
   <si>
     <t>Category</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -684,46 +684,49 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>WR02X</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>WALSIN</t>
+  </si>
+  <si>
+    <t>WR04X</t>
+  </si>
+  <si>
+    <t>WR06X</t>
+  </si>
+  <si>
     <t>Prefix</t>
-  </si>
-  <si>
-    <t>Rating_Value</t>
-  </si>
-  <si>
-    <t>Rating_Unit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Vendor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Priority</t>
-  </si>
-  <si>
-    <t>WR02X</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>WALSIN</t>
-  </si>
-  <si>
-    <t>WR04X</t>
-  </si>
-  <si>
-    <t>WR06X</t>
-  </si>
-  <si>
-    <t>CRCW0</t>
-  </si>
-  <si>
-    <t>VISHAY</t>
-  </si>
-  <si>
-    <t>ERJ2G</t>
-  </si>
-  <si>
-    <t>PANASONIC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WR25X</t>
+  </si>
+  <si>
+    <t>WR20X</t>
+  </si>
+  <si>
+    <t>WR18</t>
+  </si>
+  <si>
+    <t>WR10X</t>
+  </si>
+  <si>
+    <t>WR12X</t>
+  </si>
+  <si>
+    <t>WR08X</t>
   </si>
 </sst>
 </file>
@@ -1113,7 +1116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08DFA35F-C35F-402D-A757-AEE3B3DD27ED}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1121,33 +1124,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="B1" t="s">
-        <v>193</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>194</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1155,16 +1158,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B3">
-        <v>0.125</v>
+        <v>0.75</v>
       </c>
       <c r="C3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1172,16 +1175,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B4">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1189,19 +1192,19 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C5" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D5" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1209,16 +1212,84 @@
         <v>204</v>
       </c>
       <c r="B6">
+        <v>0.25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>205</v>
+      </c>
+      <c r="B7">
+        <v>0.125</v>
+      </c>
+      <c r="C7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B8">
         <v>0.1</v>
       </c>
-      <c r="C6" t="s">
-        <v>198</v>
-      </c>
-      <c r="D6" t="s">
-        <v>205</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
+      <c r="C8" t="s">
+        <v>193</v>
+      </c>
+      <c r="D8" t="s">
+        <v>194</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B9">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B10">
+        <v>0.05</v>
+      </c>
+      <c r="C10" t="s">
+        <v>193</v>
+      </c>
+      <c r="D10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>